<commit_message>
importando resultados para planilha
</commit_message>
<xml_diff>
--- a/Planilha de Resultados.xlsx
+++ b/Planilha de Resultados.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,6 +436,176 @@
       <c r="C1" t="inlineStr">
         <is>
           <t>Link</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2022-05-12</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Comparação entre aumento da gasolina e patrimônio da família Bolsonaro usa dados imprecisos</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>https://projetocomprova.com.br/publica%C3%A7%C3%B5es/comparacao-entre-aumento-da-gasolina-e-patrimonio-da-familia-bolsonaro-usa-dados-imprecisos/</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2022-05-12</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Publicação que atribui a ex-tesoureiro do PT áudio contra igrejas é montagem</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>https://projetocomprova.com.br/publica%C3%A7%C3%B5es/publicacao-que-atribui-a-ex-tesoureiro-do-pt-audio-contra-igrejas-e-montagem/</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2022-05-10</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>É enganoso e está fora de contexto vídeo no TikTok em que Lula chama colaborador da Petrobras de corrupto</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>https://projetocomprova.com.br/publica%C3%A7%C3%B5es/e-enganoso-e-esta-fora-de-contexto-video-no-tiktok-em-que-lula-chama-colaborador-da-petrobras-de-corrupto/</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2022-05-09</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Jovem que faz sátira sobre militantes de esquerda não é filha da deputada Maria do Rosário</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>https://projetocomprova.com.br/publica%C3%A7%C3%B5es/jovem-que-faz-satira-sobre-militantes-de-esquerda-nao-e-filha-da-deputada-maria-do-rosario/</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2022-05-06</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Publicação tira de contexto declarações de Djavan para atacar a Lei Rouanet</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>https://projetocomprova.com.br/publica%C3%A7%C3%B5es/publicacao-tira-de-contexto-declaracoes-de-djavan-para-atacar-a-lei-rouanet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2022-05-05</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Protesto de indígenas na Bahia era por melhoria na educação e não por verba para ato contra Bolsonaro</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>https://projetocomprova.com.br/publica%C3%A7%C3%B5es/protesto-de-indigenas-na-bahia-era-por-melhoria-na-educacao-e-nao-por-verba-para-ato-contra-bolsonaro/</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2022-05-04</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Vídeos antigos são usados para enganar sobre adesão a atos pró-Bolsonaro em 1º de Maio</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>https://projetocomprova.com.br/publica%C3%A7%C3%B5es/videos-antigos-sao-usados-para-enganar-sobre-adesao-a-atos-pro-bolsonaro-em-1o-de-maio/</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2022-05-03</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Antes de ser preso, João de Deus compareceu à posse de Rosa Weber no TSE</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>https://projetocomprova.com.br/publica%C3%A7%C3%B5es/antes-de-ser-preso-joao-de-deus-compareceu-a-posse-de-rosa-weber-no-tse/</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2022-05-03</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>É falso que Elon Musk tenha citado as motociatas de Bolsonaro em entrevista na Alemanha</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>https://projetocomprova.com.br/publica%C3%A7%C3%B5es/e-falso-que-elon-musk-tenha-citado-as-motociatas-de-bolsonaro-em-entrevista-na-alemanha/</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2022-04-28</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Post confunde dados e engana sobre conflitos no campo no governo Bolsonaro</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>https://projetocomprova.com.br/publica%C3%A7%C3%B5es/post-confunde-dados-e-engana-sobre-conflitos-no-campo-no-governo-bolsonaro/</t>
         </is>
       </c>
     </row>

</xml_diff>